<commit_message>
change data driven for cases manual
</commit_message>
<xml_diff>
--- a/Data/Sheet Metal Part/Order/Order Information (SMP).xlsx
+++ b/Data/Sheet Metal Part/Order/Order Information (SMP).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation Project\gocad-automation-katalon\Data\Sheet Metal Part\Order\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8369C9D0-9B73-4278-A227-FC0947E2407D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D92CDC39-F707-43C2-95B3-630BCB132147}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="495" windowWidth="28800" windowHeight="16425" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="495" windowWidth="28800" windowHeight="16425" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FPA011" sheetId="7" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="76">
   <si>
     <t>fileName</t>
   </si>
@@ -918,7 +918,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DBA0BF0-0221-405C-9926-91F4A4D5B9A2}">
   <dimension ref="A1:R5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
@@ -1223,11 +1223,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DD295A4-7888-4573-887A-A63AAC48719B}">
-  <dimension ref="A1:R5"/>
+  <dimension ref="A1:R3"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -1313,7 +1311,7 @@
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3">
-        <v>2</v>
+        <v>1000</v>
       </c>
       <c r="D2" s="3">
         <v>3</v>
@@ -1367,7 +1365,7 @@
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3">
-        <v>1</v>
+        <v>1000</v>
       </c>
       <c r="D3" s="3">
         <v>1</v>
@@ -1412,114 +1410,6 @@
         <v>60</v>
       </c>
       <c r="R3" s="4" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18">
-      <c r="A4" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3">
-        <v>0</v>
-      </c>
-      <c r="D4" s="3">
-        <v>1</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="I4" s="3">
-        <v>1</v>
-      </c>
-      <c r="J4" s="3">
-        <v>1</v>
-      </c>
-      <c r="K4" s="3">
-        <v>1</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="M4" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="N4" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="O4" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="P4" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="Q4" s="3">
-        <v>60</v>
-      </c>
-      <c r="R4" s="4" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18">
-      <c r="A5" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3">
-        <v>0</v>
-      </c>
-      <c r="D5" s="3">
-        <v>1</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="I5" s="3">
-        <v>1</v>
-      </c>
-      <c r="J5" s="3">
-        <v>1</v>
-      </c>
-      <c r="K5" s="3">
-        <v>1</v>
-      </c>
-      <c r="L5" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="M5" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="N5" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="O5" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="P5" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="Q5" s="3">
-        <v>60</v>
-      </c>
-      <c r="R5" s="4" t="s">
         <v>69</v>
       </c>
     </row>
@@ -1661,7 +1551,7 @@
       </c>
       <c r="O2" s="4">
         <f ca="1">Calculate!$C$2</f>
-        <v>45349</v>
+        <v>45350</v>
       </c>
       <c r="P2" s="3" t="s">
         <v>63</v>
@@ -1719,7 +1609,7 @@
       </c>
       <c r="O3" s="4">
         <f ca="1">Calculate!$C$2</f>
-        <v>45349</v>
+        <v>45350</v>
       </c>
       <c r="P3" s="3" t="s">
         <v>65</v>
@@ -1777,7 +1667,7 @@
       </c>
       <c r="O4" s="4">
         <f ca="1">Calculate!$C$2</f>
-        <v>45349</v>
+        <v>45350</v>
       </c>
       <c r="P4" s="3" t="s">
         <v>67</v>
@@ -1835,7 +1725,7 @@
       </c>
       <c r="O5" s="4">
         <f ca="1">Calculate!$C$2</f>
-        <v>45349</v>
+        <v>45350</v>
       </c>
       <c r="P5" s="3" t="s">
         <v>63</v>
@@ -2557,14 +2447,14 @@
     <row r="2" spans="1:3">
       <c r="A2" s="9">
         <f ca="1">TODAY()</f>
-        <v>45196</v>
+        <v>45197</v>
       </c>
       <c r="B2" s="8">
         <v>5</v>
       </c>
       <c r="C2" s="10">
         <f ca="1">DATE(YEAR(A2),MONTH(A2)+B2,MIN(DAY(A2),DAY(DATE(YEAR(A2),MONTH(A2)+B2+1,0))))</f>
-        <v>45349</v>
+        <v>45350</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
optimize and fix issues STMI009, STMI014
</commit_message>
<xml_diff>
--- a/Data/Sheet Metal Part/Order/Order Information (SMP).xlsx
+++ b/Data/Sheet Metal Part/Order/Order Information (SMP).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation Project\gocad-automation-katalon\Data\Sheet Metal Part\Order\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28888C7A-235D-4092-93D1-1729EBAC0344}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9537926-7778-4A1D-B07B-584CB2A07B36}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="495" windowWidth="28800" windowHeight="16425" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="81">
   <si>
     <t>fileName</t>
   </si>
@@ -253,9 +253,6 @@
     <t>laserMarkingChanged</t>
   </si>
   <si>
-    <t>No Lasermarking</t>
-  </si>
-  <si>
     <t>One-sided</t>
   </si>
   <si>
@@ -266,6 +263,12 @@
   </si>
   <si>
     <t>partAccordingToTheDrawing</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No </t>
   </si>
 </sst>
 </file>
@@ -275,12 +278,19 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -336,11 +346,11 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -355,7 +365,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1">
@@ -369,6 +379,9 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -654,7 +667,7 @@
   <dimension ref="A1:R5"/>
   <sheetViews>
     <sheetView topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1:K1048576"/>
+      <selection activeCell="H16" sqref="H16:H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -711,7 +724,7 @@
         <v>3</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>5</v>
@@ -750,13 +763,13 @@
         <v>25</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="H2" s="12" t="s">
-        <v>76</v>
+      <c r="H2" s="11" t="s">
+        <v>75</v>
       </c>
       <c r="I2" s="3">
         <v>4</v>
@@ -804,13 +817,13 @@
         <v>36</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="H3" s="12" t="s">
-        <v>72</v>
+      <c r="H3" s="13" t="s">
+        <v>79</v>
       </c>
       <c r="I3" s="3">
         <v>1</v>
@@ -858,13 +871,13 @@
         <v>43</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="H4" s="12" t="s">
-        <v>77</v>
+      <c r="H4" s="11" t="s">
+        <v>76</v>
       </c>
       <c r="I4" s="3">
         <v>1</v>
@@ -912,13 +925,13 @@
         <v>50</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="H5" s="12" t="s">
-        <v>78</v>
+      <c r="H5" s="11" t="s">
+        <v>77</v>
       </c>
       <c r="I5" s="3">
         <v>1</v>
@@ -961,7 +974,7 @@
   <dimension ref="A1:S5"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1:K1048576"/>
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1019,7 +1032,7 @@
         <v>3</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>5</v>
@@ -1060,14 +1073,14 @@
       <c r="E2" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="F2" s="11" t="s">
-        <v>75</v>
+      <c r="F2" s="12" t="s">
+        <v>79</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="H2" s="12" t="s">
-        <v>76</v>
+      <c r="H2" s="11" t="s">
+        <v>75</v>
       </c>
       <c r="I2" s="3">
         <v>4</v>
@@ -1117,14 +1130,14 @@
       <c r="E3" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="F3" s="11" t="s">
-        <v>75</v>
+      <c r="F3" s="12" t="s">
+        <v>79</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="H3" s="12" t="s">
-        <v>72</v>
+      <c r="H3" s="13" t="s">
+        <v>79</v>
       </c>
       <c r="I3" s="3">
         <v>1</v>
@@ -1174,14 +1187,14 @@
       <c r="E4" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="F4" s="11" t="s">
-        <v>75</v>
+      <c r="F4" s="12" t="s">
+        <v>79</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="H4" s="12" t="s">
-        <v>77</v>
+      <c r="H4" s="11" t="s">
+        <v>76</v>
       </c>
       <c r="I4" s="3">
         <v>1</v>
@@ -1231,14 +1244,14 @@
       <c r="E5" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="F5" s="11" t="s">
-        <v>75</v>
+      <c r="F5" s="12" t="s">
+        <v>79</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="H5" s="12" t="s">
-        <v>78</v>
+      <c r="H5" s="11" t="s">
+        <v>77</v>
       </c>
       <c r="I5" s="3">
         <v>1</v>
@@ -1285,7 +1298,7 @@
   <dimension ref="A1:S3"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M20" sqref="M20"/>
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1343,7 +1356,7 @@
         <v>3</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>5</v>
@@ -1384,14 +1397,14 @@
       <c r="E2" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="F2" s="11" t="s">
-        <v>75</v>
+      <c r="F2" s="12" t="s">
+        <v>79</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="H2" s="12" t="s">
-        <v>76</v>
+      <c r="H2" s="11" t="s">
+        <v>75</v>
       </c>
       <c r="I2" s="3">
         <v>4</v>
@@ -1399,7 +1412,7 @@
       <c r="J2" s="3">
         <v>5</v>
       </c>
-      <c r="K2" s="12" t="s">
+      <c r="K2" s="11" t="s">
         <v>27</v>
       </c>
       <c r="L2" s="3">
@@ -1441,14 +1454,14 @@
       <c r="E3" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="F3" s="11" t="s">
-        <v>75</v>
+      <c r="F3" s="12" t="s">
+        <v>79</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="H3" s="12" t="s">
-        <v>72</v>
+      <c r="H3" s="13" t="s">
+        <v>79</v>
       </c>
       <c r="I3" s="3">
         <v>1</v>
@@ -1494,7 +1507,7 @@
   <dimension ref="A1:T5"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1:K1048576"/>
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1553,7 +1566,7 @@
         <v>3</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>5</v>
@@ -1597,14 +1610,14 @@
       <c r="E2" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="F2" s="11" t="s">
-        <v>75</v>
+      <c r="F2" s="12" t="s">
+        <v>80</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="H2" s="12" t="s">
-        <v>76</v>
+      <c r="H2" s="11" t="s">
+        <v>75</v>
       </c>
       <c r="I2" s="3">
         <v>4</v>
@@ -1629,7 +1642,7 @@
       </c>
       <c r="P2" s="4">
         <f ca="1">Calculate!$C$2</f>
-        <v>45376</v>
+        <v>45379</v>
       </c>
       <c r="Q2" s="3" t="s">
         <v>58</v>
@@ -1658,14 +1671,14 @@
       <c r="E3" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="F3" s="11" t="s">
-        <v>75</v>
+      <c r="F3" s="12" t="s">
+        <v>80</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="H3" s="12" t="s">
-        <v>72</v>
+      <c r="H3" s="13" t="s">
+        <v>79</v>
       </c>
       <c r="I3" s="3">
         <v>1</v>
@@ -1690,7 +1703,7 @@
       </c>
       <c r="P3" s="4">
         <f ca="1">Calculate!$C$2</f>
-        <v>45376</v>
+        <v>45379</v>
       </c>
       <c r="Q3" s="3" t="s">
         <v>60</v>
@@ -1719,14 +1732,14 @@
       <c r="E4" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="F4" s="11" t="s">
-        <v>75</v>
+      <c r="F4" s="12" t="s">
+        <v>80</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="H4" s="12" t="s">
-        <v>77</v>
+      <c r="H4" s="11" t="s">
+        <v>76</v>
       </c>
       <c r="I4" s="3">
         <v>1</v>
@@ -1751,7 +1764,7 @@
       </c>
       <c r="P4" s="4">
         <f ca="1">Calculate!$C$2</f>
-        <v>45376</v>
+        <v>45379</v>
       </c>
       <c r="Q4" s="3" t="s">
         <v>62</v>
@@ -1780,14 +1793,14 @@
       <c r="E5" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="F5" s="11" t="s">
-        <v>75</v>
+      <c r="F5" s="12" t="s">
+        <v>80</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="H5" s="12" t="s">
-        <v>78</v>
+      <c r="H5" s="11" t="s">
+        <v>77</v>
       </c>
       <c r="I5" s="3">
         <v>1</v>
@@ -1812,7 +1825,7 @@
       </c>
       <c r="P5" s="4">
         <f ca="1">Calculate!$C$2</f>
-        <v>45376</v>
+        <v>45379</v>
       </c>
       <c r="Q5" s="3" t="s">
         <v>58</v>
@@ -1836,8 +1849,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50AAE34D-C5F5-4479-9641-59F1F5898040}">
   <dimension ref="A1:P5"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1:K1048576"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1892,7 +1905,7 @@
         <v>3</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>5</v>
@@ -1924,14 +1937,14 @@
       <c r="E2" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="F2" s="11" t="s">
-        <v>75</v>
+      <c r="F2" s="12" t="s">
+        <v>79</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="H2" s="12" t="s">
-        <v>76</v>
+      <c r="H2" s="11" t="s">
+        <v>75</v>
       </c>
       <c r="I2" s="3">
         <v>4</v>
@@ -1972,14 +1985,14 @@
       <c r="E3" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="F3" s="11" t="s">
-        <v>75</v>
+      <c r="F3" s="12" t="s">
+        <v>79</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="H3" s="12" t="s">
-        <v>72</v>
+      <c r="H3" s="13" t="s">
+        <v>79</v>
       </c>
       <c r="I3" s="3">
         <v>1</v>
@@ -2020,14 +2033,14 @@
       <c r="E4" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="F4" s="11" t="s">
-        <v>75</v>
+      <c r="F4" s="12" t="s">
+        <v>79</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="H4" s="12" t="s">
-        <v>77</v>
+      <c r="H4" s="11" t="s">
+        <v>76</v>
       </c>
       <c r="I4" s="3">
         <v>1</v>
@@ -2068,14 +2081,14 @@
       <c r="E5" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="F5" s="11" t="s">
-        <v>75</v>
+      <c r="F5" s="12" t="s">
+        <v>79</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="H5" s="12" t="s">
-        <v>78</v>
+      <c r="H5" s="11" t="s">
+        <v>77</v>
       </c>
       <c r="I5" s="3">
         <v>1</v>
@@ -2111,8 +2124,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E08C9849-CB54-465E-AADF-08DB0E1F7827}">
   <dimension ref="A1:Z5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -2135,7 +2148,7 @@
     <col min="17" max="17" width="28.5703125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="26.85546875" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="33" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="30" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="27.140625" bestFit="1" customWidth="1"/>
     <col min="21" max="24" width="30" customWidth="1"/>
     <col min="25" max="25" width="35.42578125" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="22.85546875" bestFit="1" customWidth="1"/>
@@ -2173,7 +2186,7 @@
         <v>3</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>5</v>
@@ -2235,14 +2248,14 @@
       <c r="E2" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="F2" s="11" t="s">
-        <v>75</v>
+      <c r="F2" s="12" t="s">
+        <v>79</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="H2" s="12" t="s">
-        <v>76</v>
+      <c r="H2" s="11" t="s">
+        <v>75</v>
       </c>
       <c r="I2" s="3">
         <v>4</v>
@@ -2277,8 +2290,8 @@
       <c r="S2" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="T2" s="11" t="s">
-        <v>75</v>
+      <c r="T2" s="12" t="s">
+        <v>79</v>
       </c>
       <c r="U2" s="5" t="s">
         <v>72</v>
@@ -2313,14 +2326,14 @@
       <c r="E3" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="F3" s="11" t="s">
-        <v>75</v>
+      <c r="F3" s="12" t="s">
+        <v>79</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="H3" s="12" t="s">
-        <v>72</v>
+      <c r="H3" s="13" t="s">
+        <v>79</v>
       </c>
       <c r="I3" s="3">
         <v>1</v>
@@ -2355,8 +2368,8 @@
       <c r="S3" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="T3" s="11" t="s">
-        <v>75</v>
+      <c r="T3" s="12" t="s">
+        <v>79</v>
       </c>
       <c r="U3" s="5" t="s">
         <v>71</v>
@@ -2391,14 +2404,14 @@
       <c r="E4" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="F4" s="11" t="s">
-        <v>75</v>
+      <c r="F4" s="12" t="s">
+        <v>79</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="H4" s="12" t="s">
-        <v>77</v>
+      <c r="H4" s="11" t="s">
+        <v>76</v>
       </c>
       <c r="I4" s="3">
         <v>1</v>
@@ -2433,8 +2446,8 @@
       <c r="S4" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="T4" s="11" t="s">
-        <v>75</v>
+      <c r="T4" s="12" t="s">
+        <v>79</v>
       </c>
       <c r="U4" s="5" t="s">
         <v>72</v>
@@ -2469,14 +2482,14 @@
       <c r="E5" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="F5" s="11" t="s">
-        <v>75</v>
+      <c r="F5" s="12" t="s">
+        <v>79</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="H5" s="12" t="s">
-        <v>78</v>
+      <c r="H5" s="11" t="s">
+        <v>77</v>
       </c>
       <c r="I5" s="3">
         <v>1</v>
@@ -2511,8 +2524,8 @@
       <c r="S5" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="T5" s="11" t="s">
-        <v>75</v>
+      <c r="T5" s="12" t="s">
+        <v>79</v>
       </c>
       <c r="U5" s="5" t="s">
         <v>71</v>
@@ -2567,14 +2580,14 @@
     <row r="2" spans="1:3">
       <c r="A2" s="9">
         <f ca="1">TODAY()</f>
-        <v>45224</v>
+        <v>45227</v>
       </c>
       <c r="B2" s="8">
         <v>5</v>
       </c>
       <c r="C2" s="10">
         <f ca="1">DATE(YEAR(A2),MONTH(A2)+B2,MIN(DAY(A2),DAY(DATE(YEAR(A2),MONTH(A2)+B2+1,0))))</f>
-        <v>45376</v>
+        <v>45379</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new fix change UI
</commit_message>
<xml_diff>
--- a/Data/Sheet Metal Part/Order/Order Information (SMP).xlsx
+++ b/Data/Sheet Metal Part/Order/Order Information (SMP).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation Project\gocad-automation-katalon\Data\Sheet Metal Part\Order\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9537926-7778-4A1D-B07B-584CB2A07B36}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7B8737D-508D-4336-9341-FA8C695A06AB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="495" windowWidth="28800" windowHeight="16425" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="495" windowWidth="28800" windowHeight="16425" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FPA011" sheetId="7" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="82">
   <si>
     <t>fileName</t>
   </si>
@@ -269,6 +269,9 @@
   </si>
   <si>
     <t xml:space="preserve">No </t>
+  </si>
+  <si>
+    <t>X2CrNiMo17</t>
   </si>
 </sst>
 </file>
@@ -666,8 +669,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4639641D-1D4F-4B71-AC19-D76CD20CBA7F}">
   <dimension ref="A1:R5"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16:H17"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -787,7 +790,7 @@
         <v>8</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>28</v>
+        <v>81</v>
       </c>
       <c r="O2" s="5" t="s">
         <v>24</v>
@@ -974,7 +977,7 @@
   <dimension ref="A1:S5"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+      <selection activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1068,7 +1071,7 @@
         <v>2</v>
       </c>
       <c r="D2" s="3">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>25</v>
@@ -1098,7 +1101,7 @@
         <v>8</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>28</v>
+        <v>81</v>
       </c>
       <c r="O2" s="5" t="s">
         <v>24</v>
@@ -1125,7 +1128,7 @@
         <v>1</v>
       </c>
       <c r="D3" s="3">
-        <v>60</v>
+        <v>11</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>36</v>
@@ -1182,7 +1185,7 @@
         <v>0</v>
       </c>
       <c r="D4" s="3">
-        <v>40</v>
+        <v>12</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>43</v>
@@ -1239,7 +1242,7 @@
         <v>0</v>
       </c>
       <c r="D5" s="3">
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>50</v>
@@ -1642,7 +1645,7 @@
       </c>
       <c r="P2" s="4">
         <f ca="1">Calculate!$C$2</f>
-        <v>45379</v>
+        <v>45386</v>
       </c>
       <c r="Q2" s="3" t="s">
         <v>58</v>
@@ -1703,7 +1706,7 @@
       </c>
       <c r="P3" s="4">
         <f ca="1">Calculate!$C$2</f>
-        <v>45379</v>
+        <v>45386</v>
       </c>
       <c r="Q3" s="3" t="s">
         <v>60</v>
@@ -1764,7 +1767,7 @@
       </c>
       <c r="P4" s="4">
         <f ca="1">Calculate!$C$2</f>
-        <v>45379</v>
+        <v>45386</v>
       </c>
       <c r="Q4" s="3" t="s">
         <v>62</v>
@@ -1825,7 +1828,7 @@
       </c>
       <c r="P5" s="4">
         <f ca="1">Calculate!$C$2</f>
-        <v>45379</v>
+        <v>45386</v>
       </c>
       <c r="Q5" s="3" t="s">
         <v>58</v>
@@ -2124,7 +2127,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E08C9849-CB54-465E-AADF-08DB0E1F7827}">
   <dimension ref="A1:Z5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
@@ -2580,14 +2583,14 @@
     <row r="2" spans="1:3">
       <c r="A2" s="9">
         <f ca="1">TODAY()</f>
-        <v>45227</v>
+        <v>45234</v>
       </c>
       <c r="B2" s="8">
         <v>5</v>
       </c>
       <c r="C2" s="10">
         <f ca="1">DATE(YEAR(A2),MONTH(A2)+B2,MIN(DAY(A2),DAY(DATE(YEAR(A2),MONTH(A2)+B2+1,0))))</f>
-        <v>45379</v>
+        <v>45386</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
change config data driven
</commit_message>
<xml_diff>
--- a/Data/Sheet Metal Part/Order/Order Information (SMP).xlsx
+++ b/Data/Sheet Metal Part/Order/Order Information (SMP).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation Project\gocad-automation-katalon\Data\Sheet Metal Part\Order\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{302A02CF-2072-4ADC-B8BC-859DF8A60E44}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{257476C9-1E4B-45B1-89AC-05E179A0AA6C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="495" windowWidth="28800" windowHeight="16425" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="495" windowWidth="28800" windowHeight="16425" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FPA011" sheetId="7" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="81">
   <si>
     <t>fileName</t>
   </si>
@@ -260,9 +260,6 @@
   </si>
   <si>
     <t>Two-sided</t>
-  </si>
-  <si>
-    <t>partAccordingToTheDrawing</t>
   </si>
   <si>
     <t>No</t>
@@ -667,10 +664,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4639641D-1D4F-4B71-AC19-D76CD20CBA7F}">
-  <dimension ref="A1:R5"/>
+  <dimension ref="A1:Q5"/>
   <sheetViews>
     <sheetView topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N17" sqref="N17"/>
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -685,17 +682,16 @@
     <col min="8" max="8" width="22" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="20.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="26.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="19.140625" customWidth="1"/>
-    <col min="17" max="17" width="40.28515625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="31.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19.140625" customWidth="1"/>
+    <col min="16" max="16" width="40.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="31.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:17">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -727,31 +723,28 @@
         <v>3</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>78</v>
+        <v>5</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>10</v>
+        <v>56</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="R1" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:18">
+    <row r="2" spans="1:17">
       <c r="A2" s="3" t="s">
         <v>33</v>
       </c>
@@ -766,7 +759,7 @@
         <v>25</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>26</v>
@@ -780,32 +773,29 @@
       <c r="J2" s="3">
         <v>5</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="K2" s="3">
+        <v>6</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="N2" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="L2" s="3">
-        <v>6</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="O2" s="5" t="s">
-        <v>24</v>
+      <c r="O2" s="3" t="s">
+        <v>58</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="Q2" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="R2" s="4" t="s">
+      <c r="Q2" s="4" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:17">
       <c r="A3" s="3" t="s">
         <v>34</v>
       </c>
@@ -820,13 +810,13 @@
         <v>36</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>26</v>
       </c>
       <c r="H3" s="13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I3" s="3">
         <v>1</v>
@@ -834,32 +824,29 @@
       <c r="J3" s="3">
         <v>1</v>
       </c>
-      <c r="K3" s="5" t="s">
+      <c r="K3" s="3">
+        <v>1</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="N3" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="L3" s="3">
-        <v>1</v>
-      </c>
-      <c r="M3" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="N3" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="O3" s="5" t="s">
-        <v>24</v>
+      <c r="O3" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="P3" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="Q3" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="R3" s="4" t="s">
+      <c r="Q3" s="4" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="4" spans="1:18">
+    <row r="4" spans="1:17">
       <c r="A4" s="3" t="s">
         <v>41</v>
       </c>
@@ -874,7 +861,7 @@
         <v>43</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>26</v>
@@ -888,32 +875,29 @@
       <c r="J4" s="3">
         <v>1</v>
       </c>
-      <c r="K4" s="5" t="s">
+      <c r="K4" s="3">
+        <v>1</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="N4" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="L4" s="3">
-        <v>1</v>
-      </c>
-      <c r="M4" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="N4" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="O4" s="5" t="s">
-        <v>27</v>
+      <c r="O4" s="3" t="s">
+        <v>62</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q4" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="R4" s="4" t="s">
+      <c r="Q4" s="4" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="5" spans="1:18">
+    <row r="5" spans="1:17">
       <c r="A5" s="3" t="s">
         <v>48</v>
       </c>
@@ -928,7 +912,7 @@
         <v>50</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>26</v>
@@ -942,28 +926,25 @@
       <c r="J5" s="3">
         <v>1</v>
       </c>
-      <c r="K5" s="5" t="s">
+      <c r="K5" s="3">
+        <v>1</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="N5" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="L5" s="3">
-        <v>1</v>
-      </c>
-      <c r="M5" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="N5" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="O5" s="5" t="s">
-        <v>27</v>
+      <c r="O5" s="3" t="s">
+        <v>58</v>
       </c>
       <c r="P5" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="Q5" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="R5" s="4" t="s">
+      <c r="Q5" s="4" t="s">
         <v>64</v>
       </c>
     </row>
@@ -974,10 +955,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DBA0BF0-0221-405C-9926-91F4A4D5B9A2}">
-  <dimension ref="A1:S5"/>
+  <dimension ref="A1:R5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -992,18 +973,17 @@
     <col min="8" max="8" width="22" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="26.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="19.140625" customWidth="1"/>
-    <col min="17" max="17" width="38.28515625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="31.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19.140625" customWidth="1"/>
+    <col min="16" max="16" width="38.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="31.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19">
+    <row r="1" spans="1:18">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1035,34 +1015,31 @@
         <v>3</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>78</v>
+        <v>5</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>10</v>
+        <v>56</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>57</v>
+        <v>9</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="S1" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:19">
+    <row r="2" spans="1:18">
       <c r="A2" s="3" t="s">
         <v>33</v>
       </c>
@@ -1077,7 +1054,7 @@
         <v>25</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>26</v>
@@ -1091,35 +1068,32 @@
       <c r="J2" s="3">
         <v>5</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="K2" s="3">
+        <v>6</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="N2" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="L2" s="3">
-        <v>6</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="O2" s="5" t="s">
-        <v>24</v>
+      <c r="O2" s="3" t="s">
+        <v>58</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="Q2" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="R2" s="3">
+      <c r="Q2" s="3">
         <v>60</v>
       </c>
-      <c r="S2" s="4" t="s">
+      <c r="R2" s="4" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="3" spans="1:19">
+    <row r="3" spans="1:18">
       <c r="A3" s="3" t="s">
         <v>34</v>
       </c>
@@ -1134,13 +1108,13 @@
         <v>36</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>26</v>
       </c>
       <c r="H3" s="13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I3" s="3">
         <v>1</v>
@@ -1148,35 +1122,32 @@
       <c r="J3" s="3">
         <v>1</v>
       </c>
-      <c r="K3" s="5" t="s">
+      <c r="K3" s="3">
+        <v>1</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="N3" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="L3" s="3">
-        <v>1</v>
-      </c>
-      <c r="M3" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="N3" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="O3" s="5" t="s">
-        <v>24</v>
+      <c r="O3" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="P3" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q3" s="3">
         <v>60</v>
       </c>
-      <c r="Q3" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="R3" s="3">
-        <v>60</v>
-      </c>
-      <c r="S3" s="4" t="s">
+      <c r="R3" s="4" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="4" spans="1:19">
+    <row r="4" spans="1:18">
       <c r="A4" s="3" t="s">
         <v>41</v>
       </c>
@@ -1191,7 +1162,7 @@
         <v>43</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>26</v>
@@ -1205,35 +1176,32 @@
       <c r="J4" s="3">
         <v>1</v>
       </c>
-      <c r="K4" s="5" t="s">
+      <c r="K4" s="3">
+        <v>1</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="N4" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="L4" s="3">
-        <v>1</v>
-      </c>
-      <c r="M4" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="N4" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="O4" s="5" t="s">
-        <v>27</v>
+      <c r="O4" s="3" t="s">
+        <v>62</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q4" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="R4" s="3">
+      <c r="Q4" s="3">
         <v>60</v>
       </c>
-      <c r="S4" s="4" t="s">
+      <c r="R4" s="4" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="5" spans="1:19">
+    <row r="5" spans="1:18">
       <c r="A5" s="3" t="s">
         <v>48</v>
       </c>
@@ -1248,7 +1216,7 @@
         <v>50</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>26</v>
@@ -1262,31 +1230,28 @@
       <c r="J5" s="3">
         <v>1</v>
       </c>
-      <c r="K5" s="5" t="s">
+      <c r="K5" s="3">
+        <v>1</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="N5" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="L5" s="3">
-        <v>1</v>
-      </c>
-      <c r="M5" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="N5" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="O5" s="5" t="s">
-        <v>27</v>
+      <c r="O5" s="3" t="s">
+        <v>58</v>
       </c>
       <c r="P5" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="Q5" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="R5" s="3">
+      <c r="Q5" s="3">
         <v>60</v>
       </c>
-      <c r="S5" s="4" t="s">
+      <c r="R5" s="4" t="s">
         <v>64</v>
       </c>
     </row>
@@ -1298,7 +1263,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DD295A4-7888-4573-887A-A63AAC48719B}">
-  <dimension ref="A1:S3"/>
+  <dimension ref="A1:R3"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="H23" sqref="H23"/>
@@ -1316,18 +1281,17 @@
     <col min="8" max="8" width="22" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="26.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="19.140625" customWidth="1"/>
-    <col min="17" max="17" width="38.28515625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="31.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19.140625" customWidth="1"/>
+    <col min="16" max="16" width="38.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="31.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19">
+    <row r="1" spans="1:18">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1359,34 +1323,31 @@
         <v>3</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>78</v>
+        <v>5</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>10</v>
+        <v>56</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>57</v>
+        <v>9</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="S1" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:19">
+    <row r="2" spans="1:18">
       <c r="A2" s="3" t="s">
         <v>33</v>
       </c>
@@ -1401,7 +1362,7 @@
         <v>25</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>26</v>
@@ -1415,35 +1376,32 @@
       <c r="J2" s="3">
         <v>5</v>
       </c>
-      <c r="K2" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="L2" s="3">
+      <c r="K2" s="3">
         <v>6</v>
       </c>
+      <c r="L2" s="3" t="s">
+        <v>8</v>
+      </c>
       <c r="M2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="N2" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="O2" s="5" t="s">
+      <c r="N2" s="5" t="s">
         <v>24</v>
       </c>
+      <c r="O2" s="3" t="s">
+        <v>58</v>
+      </c>
       <c r="P2" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="Q2" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="R2" s="3">
+      <c r="Q2" s="3">
         <v>60</v>
       </c>
-      <c r="S2" s="4" t="s">
+      <c r="R2" s="4" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="3" spans="1:19">
+    <row r="3" spans="1:18">
       <c r="A3" s="3" t="s">
         <v>34</v>
       </c>
@@ -1458,13 +1416,13 @@
         <v>36</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>26</v>
       </c>
       <c r="H3" s="13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I3" s="3">
         <v>1</v>
@@ -1472,31 +1430,28 @@
       <c r="J3" s="3">
         <v>1</v>
       </c>
-      <c r="K3" s="5" t="s">
+      <c r="K3" s="3">
+        <v>1</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="N3" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="L3" s="3">
-        <v>1</v>
-      </c>
-      <c r="M3" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="N3" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="O3" s="5" t="s">
-        <v>24</v>
+      <c r="O3" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="P3" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q3" s="3">
         <v>60</v>
       </c>
-      <c r="Q3" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="R3" s="3">
-        <v>60</v>
-      </c>
-      <c r="S3" s="4" t="s">
+      <c r="R3" s="4" t="s">
         <v>64</v>
       </c>
     </row>
@@ -1507,10 +1462,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{147B69C7-A702-45C4-913D-71E1B6AF4D13}">
-  <dimension ref="A1:T5"/>
+  <dimension ref="A1:S5"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+      <selection activeCell="M33" sqref="M33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1525,19 +1480,18 @@
     <col min="8" max="8" width="21" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="26.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="19.140625" customWidth="1"/>
-    <col min="18" max="18" width="38.28515625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="31.28515625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="19.140625" customWidth="1"/>
+    <col min="17" max="17" width="38.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="31.28515625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="28.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1" spans="1:19">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1569,37 +1523,34 @@
         <v>3</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>78</v>
+        <v>5</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>10</v>
+        <v>70</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="S1" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="T1" s="6" t="s">
+      <c r="S1" s="6" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:20">
+    <row r="2" spans="1:19">
       <c r="A2" s="3" t="s">
         <v>33</v>
       </c>
@@ -1614,7 +1565,7 @@
         <v>25</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>26</v>
@@ -1628,39 +1579,36 @@
       <c r="J2" s="3">
         <v>5</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="K2" s="3">
+        <v>6</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="N2" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="L2" s="3">
-        <v>6</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="O2" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="P2" s="4">
+      <c r="O2" s="4">
         <f ca="1">Calculate!$C$2</f>
-        <v>45389</v>
+        <v>45398</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>58</v>
       </c>
       <c r="Q2" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="R2" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="S2" s="4" t="s">
+      <c r="R2" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="T2" s="7" t="s">
+      <c r="S2" s="7" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="3" spans="1:20">
+    <row r="3" spans="1:19">
       <c r="A3" s="3" t="s">
         <v>34</v>
       </c>
@@ -1675,13 +1623,13 @@
         <v>36</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>26</v>
       </c>
       <c r="H3" s="13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I3" s="3">
         <v>1</v>
@@ -1689,39 +1637,36 @@
       <c r="J3" s="3">
         <v>1</v>
       </c>
-      <c r="K3" s="5" t="s">
+      <c r="K3" s="3">
+        <v>1</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="N3" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="L3" s="3">
-        <v>1</v>
-      </c>
-      <c r="M3" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="N3" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="O3" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="P3" s="4">
+      <c r="O3" s="4">
         <f ca="1">Calculate!$C$2</f>
-        <v>45389</v>
+        <v>45398</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="Q3" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="R3" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="S3" s="4" t="s">
+      <c r="R3" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="T3" s="7" t="s">
+      <c r="S3" s="7" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="4" spans="1:20">
+    <row r="4" spans="1:19">
       <c r="A4" s="3" t="s">
         <v>41</v>
       </c>
@@ -1736,7 +1681,7 @@
         <v>43</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>26</v>
@@ -1750,39 +1695,36 @@
       <c r="J4" s="3">
         <v>1</v>
       </c>
-      <c r="K4" s="5" t="s">
+      <c r="K4" s="3">
+        <v>1</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="N4" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="L4" s="3">
-        <v>1</v>
-      </c>
-      <c r="M4" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="N4" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="O4" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="P4" s="4">
+      <c r="O4" s="4">
         <f ca="1">Calculate!$C$2</f>
-        <v>45389</v>
+        <v>45398</v>
+      </c>
+      <c r="P4" s="3" t="s">
+        <v>62</v>
       </c>
       <c r="Q4" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="R4" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="S4" s="4" t="s">
+      <c r="R4" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="T4" s="7" t="s">
+      <c r="S4" s="7" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="5" spans="1:20">
+    <row r="5" spans="1:19">
       <c r="A5" s="3" t="s">
         <v>48</v>
       </c>
@@ -1797,7 +1739,7 @@
         <v>50</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>26</v>
@@ -1811,35 +1753,32 @@
       <c r="J5" s="3">
         <v>1</v>
       </c>
-      <c r="K5" s="5" t="s">
+      <c r="K5" s="3">
+        <v>1</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="N5" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="L5" s="3">
-        <v>1</v>
-      </c>
-      <c r="M5" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="N5" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="O5" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="P5" s="4">
+      <c r="O5" s="4">
         <f ca="1">Calculate!$C$2</f>
-        <v>45389</v>
+        <v>45398</v>
+      </c>
+      <c r="P5" s="3" t="s">
+        <v>58</v>
       </c>
       <c r="Q5" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="R5" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="S5" s="4" t="s">
+      <c r="R5" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="T5" s="7" t="s">
+      <c r="S5" s="7" t="s">
         <v>66</v>
       </c>
     </row>
@@ -1850,10 +1789,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50AAE34D-C5F5-4479-9641-59F1F5898040}">
-  <dimension ref="A1:P5"/>
+  <dimension ref="A1:O5"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H31" sqref="H31"/>
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1868,15 +1807,14 @@
     <col min="8" max="8" width="22" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="20.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="26.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1908,25 +1846,22 @@
         <v>3</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>78</v>
+        <v>5</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="P1" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:15">
       <c r="A2" s="3" t="s">
         <v>33</v>
       </c>
@@ -1941,7 +1876,7 @@
         <v>25</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>26</v>
@@ -1955,26 +1890,23 @@
       <c r="J2" s="3">
         <v>5</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="K2" s="3">
+        <v>6</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="N2" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="L2" s="3">
-        <v>6</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="O2" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="P2" s="4" t="s">
+      <c r="O2" s="4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:15">
       <c r="A3" s="3" t="s">
         <v>34</v>
       </c>
@@ -1989,13 +1921,13 @@
         <v>36</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>26</v>
       </c>
       <c r="H3" s="13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I3" s="3">
         <v>1</v>
@@ -2003,26 +1935,23 @@
       <c r="J3" s="3">
         <v>1</v>
       </c>
-      <c r="K3" s="5" t="s">
+      <c r="K3" s="3">
+        <v>1</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="N3" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="L3" s="3">
-        <v>1</v>
-      </c>
-      <c r="M3" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="N3" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="O3" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="P3" s="4" t="s">
+      <c r="O3" s="4" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:15">
       <c r="A4" s="3" t="s">
         <v>41</v>
       </c>
@@ -2037,7 +1966,7 @@
         <v>43</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>26</v>
@@ -2051,26 +1980,23 @@
       <c r="J4" s="3">
         <v>1</v>
       </c>
-      <c r="K4" s="5" t="s">
+      <c r="K4" s="3">
+        <v>1</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="N4" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="L4" s="3">
-        <v>1</v>
-      </c>
-      <c r="M4" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="N4" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="O4" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="P4" s="4" t="s">
+      <c r="O4" s="4" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:15">
       <c r="A5" s="3" t="s">
         <v>48</v>
       </c>
@@ -2085,7 +2011,7 @@
         <v>50</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>26</v>
@@ -2099,22 +2025,19 @@
       <c r="J5" s="3">
         <v>1</v>
       </c>
-      <c r="K5" s="5" t="s">
+      <c r="K5" s="3">
+        <v>1</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="N5" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="L5" s="3">
-        <v>1</v>
-      </c>
-      <c r="M5" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="N5" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="O5" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="P5" s="4" t="s">
+      <c r="O5" s="4" t="s">
         <v>51</v>
       </c>
     </row>
@@ -2125,10 +2048,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E08C9849-CB54-465E-AADF-08DB0E1F7827}">
-  <dimension ref="A1:Z5"/>
+  <dimension ref="A1:Y5"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="N22" sqref="N22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -2142,22 +2065,21 @@
     <col min="7" max="8" width="16.85546875" customWidth="1"/>
     <col min="9" max="9" width="20.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="26.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="28.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="26.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="33" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="27.140625" bestFit="1" customWidth="1"/>
-    <col min="21" max="24" width="30" customWidth="1"/>
-    <col min="25" max="25" width="35.42578125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="33" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="23" width="30" customWidth="1"/>
+    <col min="24" max="24" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="22.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="2" customFormat="1">
+    <row r="1" spans="1:25" s="2" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2189,55 +2111,52 @@
         <v>3</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>78</v>
+        <v>5</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>19</v>
+        <v>74</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>74</v>
+        <v>20</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="Z1" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:26">
+    <row r="2" spans="1:25">
       <c r="A2" s="3" t="s">
         <v>33</v>
       </c>
@@ -2252,7 +2171,7 @@
         <v>25</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>26</v>
@@ -2266,56 +2185,53 @@
       <c r="J2" s="3">
         <v>5</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="K2" s="3">
+        <v>6</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="N2" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="L2" s="3">
+      <c r="O2" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="P2" s="3">
+        <v>4</v>
+      </c>
+      <c r="Q2" s="3">
+        <v>8</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="S2" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="T2" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="U2" s="3">
         <v>6</v>
       </c>
-      <c r="M2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="O2" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="P2" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q2" s="3">
-        <v>4</v>
-      </c>
-      <c r="R2" s="3">
-        <v>8</v>
-      </c>
-      <c r="S2" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="T2" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="U2" s="5" t="s">
-        <v>72</v>
-      </c>
       <c r="V2" s="3">
-        <v>6</v>
-      </c>
-      <c r="W2" s="3">
         <v>7</v>
       </c>
-      <c r="X2" s="3" t="s">
+      <c r="W2" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="Y2" s="5" t="s">
+      <c r="X2" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="Z2" s="3" t="s">
+      <c r="Y2" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:26">
+    <row r="3" spans="1:25">
       <c r="A3" s="3" t="s">
         <v>34</v>
       </c>
@@ -2330,13 +2246,13 @@
         <v>36</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>26</v>
       </c>
       <c r="H3" s="13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I3" s="3">
         <v>1</v>
@@ -2344,56 +2260,53 @@
       <c r="J3" s="3">
         <v>1</v>
       </c>
-      <c r="K3" s="5" t="s">
+      <c r="K3" s="3">
+        <v>1</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="N3" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="L3" s="3">
-        <v>1</v>
-      </c>
-      <c r="M3" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="N3" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="O3" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="P3" s="4" t="s">
+      <c r="O3" s="4" t="s">
         <v>37</v>
       </c>
+      <c r="P3" s="3">
+        <v>3</v>
+      </c>
       <c r="Q3" s="3">
-        <v>3</v>
-      </c>
-      <c r="R3" s="3">
-        <v>1</v>
-      </c>
-      <c r="S3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="R3" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="T3" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="U3" s="5" t="s">
+      <c r="S3" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="T3" s="5" t="s">
         <v>71</v>
       </c>
+      <c r="U3" s="3">
+        <v>4</v>
+      </c>
       <c r="V3" s="3">
-        <v>4</v>
-      </c>
-      <c r="W3" s="3">
         <v>5</v>
       </c>
-      <c r="X3" s="3" t="s">
+      <c r="W3" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="Y3" s="5" t="s">
+      <c r="X3" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="Z3" s="3" t="s">
+      <c r="Y3" s="3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:26">
+    <row r="4" spans="1:25">
       <c r="A4" s="3" t="s">
         <v>41</v>
       </c>
@@ -2408,7 +2321,7 @@
         <v>43</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>26</v>
@@ -2422,56 +2335,53 @@
       <c r="J4" s="3">
         <v>1</v>
       </c>
-      <c r="K4" s="5" t="s">
+      <c r="K4" s="3">
+        <v>1</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="N4" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="L4" s="3">
-        <v>1</v>
-      </c>
-      <c r="M4" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="N4" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="O4" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="P4" s="4" t="s">
+      <c r="O4" s="4" t="s">
         <v>45</v>
       </c>
+      <c r="P4" s="3">
+        <v>0</v>
+      </c>
       <c r="Q4" s="3">
-        <v>0</v>
-      </c>
-      <c r="R4" s="3">
         <v>2</v>
       </c>
-      <c r="S4" s="3" t="s">
+      <c r="R4" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="T4" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="U4" s="5" t="s">
+      <c r="S4" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="T4" s="5" t="s">
         <v>72</v>
       </c>
+      <c r="U4" s="3">
+        <v>5</v>
+      </c>
       <c r="V4" s="3">
-        <v>5</v>
-      </c>
-      <c r="W4" s="3">
         <v>6</v>
       </c>
-      <c r="X4" s="3" t="s">
+      <c r="W4" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="Y4" s="5" t="s">
+      <c r="X4" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="Z4" s="3" t="s">
+      <c r="Y4" s="3" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:26">
+    <row r="5" spans="1:25">
       <c r="A5" s="3" t="s">
         <v>48</v>
       </c>
@@ -2486,7 +2396,7 @@
         <v>50</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>26</v>
@@ -2500,52 +2410,49 @@
       <c r="J5" s="3">
         <v>1</v>
       </c>
-      <c r="K5" s="5" t="s">
+      <c r="K5" s="3">
+        <v>1</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="N5" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="L5" s="3">
-        <v>1</v>
-      </c>
-      <c r="M5" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="N5" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="O5" s="5" t="s">
+      <c r="O5" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="P5" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="3">
+        <v>1</v>
+      </c>
+      <c r="R5" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S5" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="T5" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="U5" s="3">
+        <v>5</v>
+      </c>
+      <c r="V5" s="3">
+        <v>6</v>
+      </c>
+      <c r="W5" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="X5" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="P5" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q5" s="3">
-        <v>0</v>
-      </c>
-      <c r="R5" s="3">
-        <v>1</v>
-      </c>
-      <c r="S5" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="T5" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="U5" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="V5" s="3">
-        <v>5</v>
-      </c>
-      <c r="W5" s="3">
-        <v>6</v>
-      </c>
-      <c r="X5" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="Y5" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="Z5" s="3" t="s">
+      <c r="Y5" s="3" t="s">
         <v>54</v>
       </c>
     </row>
@@ -2583,14 +2490,14 @@
     <row r="2" spans="1:3">
       <c r="A2" s="9">
         <f ca="1">TODAY()</f>
-        <v>45237</v>
+        <v>45246</v>
       </c>
       <c r="B2" s="8">
         <v>5</v>
       </c>
       <c r="C2" s="10">
         <f ca="1">DATE(YEAR(A2),MONTH(A2)+B2,MIN(DAY(A2),DAY(DATE(YEAR(A2),MONTH(A2)+B2+1,0))))</f>
-        <v>45389</v>
+        <v>45398</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix script some change
</commit_message>
<xml_diff>
--- a/Data/Sheet Metal Part/Order/Order Information (SMP).xlsx
+++ b/Data/Sheet Metal Part/Order/Order Information (SMP).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation Project\gocad-automation-katalon\Data\Sheet Metal Part\Order\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55659630-A7AC-47E9-8573-0CB6DECB7968}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C1D3C04-54A5-43F7-B742-2A9E23700A64}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="495" windowWidth="28800" windowHeight="16425" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -253,9 +253,6 @@
     <t>100,08</t>
   </si>
   <si>
-    <t>164,55</t>
-  </si>
-  <si>
     <t>49,20</t>
   </si>
   <si>
@@ -268,10 +265,13 @@
     <t>35,56</t>
   </si>
   <si>
-    <t>179,49</t>
-  </si>
-  <si>
     <t>46,70</t>
+  </si>
+  <si>
+    <t>156,32</t>
+  </si>
+  <si>
+    <t>175,55</t>
   </si>
 </sst>
 </file>
@@ -1605,7 +1605,7 @@
       </c>
       <c r="O2" s="4">
         <f ca="1">Calculate!$C$2</f>
-        <v>45429</v>
+        <v>45432</v>
       </c>
       <c r="P2" s="3" t="s">
         <v>43</v>
@@ -1663,7 +1663,7 @@
       </c>
       <c r="O3" s="4">
         <f ca="1">Calculate!$C$2</f>
-        <v>45429</v>
+        <v>45432</v>
       </c>
       <c r="P3" s="3" t="s">
         <v>45</v>
@@ -1721,7 +1721,7 @@
       </c>
       <c r="O4" s="4">
         <f ca="1">Calculate!$C$2</f>
-        <v>45429</v>
+        <v>45432</v>
       </c>
       <c r="P4" s="3" t="s">
         <v>47</v>
@@ -1779,7 +1779,7 @@
       </c>
       <c r="O5" s="4">
         <f ca="1">Calculate!$C$2</f>
-        <v>45429</v>
+        <v>45432</v>
       </c>
       <c r="P5" s="3" t="s">
         <v>43</v>
@@ -2062,8 +2062,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E08C9849-CB54-465E-AADF-08DB0E1F7827}">
   <dimension ref="A1:Z5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="W24" sqref="W24"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="V12" sqref="V12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -2249,7 +2249,7 @@
         <v>26</v>
       </c>
       <c r="Z2" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:26">
@@ -2294,7 +2294,7 @@
         <v>23</v>
       </c>
       <c r="O3" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="P3" s="3">
         <v>3</v>
@@ -2327,7 +2327,7 @@
         <v>26</v>
       </c>
       <c r="Z3" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:26">
@@ -2372,7 +2372,7 @@
         <v>26</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="P4" s="3">
         <v>0</v>
@@ -2405,7 +2405,7 @@
         <v>23</v>
       </c>
       <c r="Z4" s="3" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="5" spans="1:26">
@@ -2450,7 +2450,7 @@
         <v>26</v>
       </c>
       <c r="O5" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="P5" s="3">
         <v>0</v>
@@ -2483,7 +2483,7 @@
         <v>26</v>
       </c>
       <c r="Z5" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -2520,14 +2520,14 @@
     <row r="2" spans="1:3">
       <c r="A2" s="9">
         <f ca="1">TODAY()</f>
-        <v>45277</v>
+        <v>45280</v>
       </c>
       <c r="B2" s="8">
         <v>5</v>
       </c>
       <c r="C2" s="10">
         <f ca="1">DATE(YEAR(A2),MONTH(A2)+B2,MIN(DAY(A2),DAY(DATE(YEAR(A2),MONTH(A2)+B2+1,0))))</f>
-        <v>45429</v>
+        <v>45432</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add new file step
</commit_message>
<xml_diff>
--- a/Data/Sheet Metal Part/Order/Order Information (SMP).xlsx
+++ b/Data/Sheet Metal Part/Order/Order Information (SMP).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation Project\gocad-automation-katalon\Data\Sheet Metal Part\Order\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAA2DC18-1C75-4957-9F64-FF382321CB1E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1F3DA27-0AC3-42E0-BB59-5B7418D8D113}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="495" windowWidth="28800" windowHeight="16425" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="495" windowWidth="28800" windowHeight="16425" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FPA011" sheetId="7" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="87">
   <si>
     <t>fileName</t>
   </si>
@@ -115,12 +115,6 @@
     <t>Soft annealing</t>
   </si>
   <si>
-    <t>dxf-testing.dxf</t>
-  </si>
-  <si>
-    <t>dwg-testing.dwg</t>
-  </si>
-  <si>
     <t>EN AW-6082 / AlMgSi1</t>
   </si>
   <si>
@@ -130,9 +124,6 @@
     <t>44,61</t>
   </si>
   <si>
-    <t>Plasma nitriding</t>
-  </si>
-  <si>
     <t>stp-testing.stp</t>
   </si>
   <si>
@@ -145,9 +136,6 @@
     <t>49,65</t>
   </si>
   <si>
-    <t>Phosphating</t>
-  </si>
-  <si>
     <t>packagingAndShippingComments</t>
   </si>
   <si>
@@ -214,12 +202,6 @@
     <t>X2CrNiMo17</t>
   </si>
   <si>
-    <t>Copper</t>
-  </si>
-  <si>
-    <t>CuSn8</t>
-  </si>
-  <si>
     <t>Stainless steel</t>
   </si>
   <si>
@@ -229,12 +211,6 @@
     <t>X5CrNi18</t>
   </si>
   <si>
-    <t>EPDM 65 Premium</t>
-  </si>
-  <si>
-    <t>Rubber</t>
-  </si>
-  <si>
     <t>EN AW-6060 / AlMgSi</t>
   </si>
   <si>
@@ -244,9 +220,6 @@
     <t>Sandblasting</t>
   </si>
   <si>
-    <t>AlMg3-Blech</t>
-  </si>
-  <si>
     <t>115,80</t>
   </si>
   <si>
@@ -305,6 +278,15 @@
   </si>
   <si>
     <t>Chromatieren</t>
+  </si>
+  <si>
+    <t>Aluminium</t>
+  </si>
+  <si>
+    <t>stp-testing 2.stp</t>
+  </si>
+  <si>
+    <t>stp-testing 3.stp</t>
   </si>
 </sst>
 </file>
@@ -713,7 +695,7 @@
   <dimension ref="A1:Q5"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2:M5"/>
+      <selection activeCell="A2" sqref="A2:A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -754,7 +736,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>11</v>
@@ -781,18 +763,18 @@
         <v>9</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:17">
       <c r="A2" s="3" t="s">
-        <v>29</v>
+        <v>85</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3">
@@ -802,16 +784,16 @@
         <v>2</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>25</v>
       </c>
       <c r="H2" s="11" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="I2" s="3">
         <v>4</v>
@@ -823,27 +805,27 @@
         <v>6</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="N2" s="5" t="s">
         <v>23</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="Q2" s="4" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:17">
       <c r="A3" s="3" t="s">
-        <v>30</v>
+        <v>86</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3">
@@ -853,16 +835,16 @@
         <v>2</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>25</v>
       </c>
       <c r="H3" s="13" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="I3" s="3">
         <v>4</v>
@@ -874,27 +856,27 @@
         <v>6</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>65</v>
+        <v>84</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="N3" s="5" t="s">
         <v>23</v>
       </c>
       <c r="O3" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q3" s="4" t="s">
         <v>45</v>
-      </c>
-      <c r="P3" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q3" s="4" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:17">
       <c r="A4" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="3">
@@ -904,16 +886,16 @@
         <v>1</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>25</v>
       </c>
       <c r="H4" s="14" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="I4" s="3">
         <v>4</v>
@@ -925,27 +907,27 @@
         <v>6</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="N4" s="5" t="s">
         <v>26</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="Q4" s="4" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:17">
       <c r="A5" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3">
@@ -955,16 +937,16 @@
         <v>1</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>25</v>
       </c>
       <c r="H5" s="11" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="I5" s="3">
         <v>4</v>
@@ -976,22 +958,22 @@
         <v>6</v>
       </c>
       <c r="L5" s="3" t="s">
-        <v>65</v>
+        <v>84</v>
       </c>
       <c r="M5" s="3" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="N5" s="5" t="s">
         <v>26</v>
       </c>
       <c r="O5" s="3" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="P5" s="3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="Q5" s="4" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -1004,8 +986,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DBA0BF0-0221-405C-9926-91F4A4D5B9A2}">
   <dimension ref="A1:S5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1048,7 +1030,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>11</v>
@@ -1075,24 +1057,24 @@
         <v>9</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="Q1" s="1" t="s">
         <v>8</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:19">
       <c r="A2" s="3" t="s">
-        <v>29</v>
+        <v>85</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3">
@@ -1102,16 +1084,16 @@
         <v>50</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>25</v>
       </c>
       <c r="H2" s="11" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="I2" s="3">
         <v>4</v>
@@ -1123,25 +1105,25 @@
         <v>6</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="N2" s="5" t="s">
         <v>23</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="Q2" s="3">
         <v>60</v>
       </c>
       <c r="R2" s="4" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="S2" s="3">
         <v>15</v>
@@ -1149,7 +1131,7 @@
     </row>
     <row r="3" spans="1:19">
       <c r="A3" s="3" t="s">
-        <v>30</v>
+        <v>86</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3">
@@ -1159,16 +1141,16 @@
         <v>500</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>25</v>
       </c>
       <c r="H3" s="13" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="I3" s="3">
         <v>1</v>
@@ -1180,25 +1162,25 @@
         <v>1</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>65</v>
+        <v>84</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="N3" s="5" t="s">
         <v>23</v>
       </c>
       <c r="O3" s="3" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="P3" s="3" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="Q3" s="3">
         <v>60</v>
       </c>
       <c r="R3" s="4" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="S3" s="3">
         <v>6</v>
@@ -1206,7 +1188,7 @@
     </row>
     <row r="4" spans="1:19">
       <c r="A4" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="3">
@@ -1216,16 +1198,16 @@
         <v>50</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>25</v>
       </c>
       <c r="H4" s="14" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="I4" s="3">
         <v>1</v>
@@ -1237,25 +1219,25 @@
         <v>1</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="N4" s="5" t="s">
         <v>26</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="Q4" s="3">
         <v>60</v>
       </c>
       <c r="R4" s="4" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="S4" s="3">
         <v>7</v>
@@ -1263,7 +1245,7 @@
     </row>
     <row r="5" spans="1:19">
       <c r="A5" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3">
@@ -1273,16 +1255,16 @@
         <v>50</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>25</v>
       </c>
       <c r="H5" s="11" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="I5" s="3">
         <v>1</v>
@@ -1294,25 +1276,25 @@
         <v>1</v>
       </c>
       <c r="L5" s="3" t="s">
-        <v>65</v>
+        <v>84</v>
       </c>
       <c r="M5" s="3" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="N5" s="5" t="s">
         <v>26</v>
       </c>
       <c r="O5" s="3" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="P5" s="3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="Q5" s="3">
         <v>60</v>
       </c>
       <c r="R5" s="4" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="S5" s="3">
         <v>15</v>
@@ -1328,7 +1310,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DD295A4-7888-4573-887A-A63AAC48719B}">
   <dimension ref="A1:R3"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -1369,7 +1353,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>11</v>
@@ -1396,21 +1380,21 @@
         <v>9</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="Q1" s="1" t="s">
         <v>8</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:18">
       <c r="A2" s="3" t="s">
-        <v>29</v>
+        <v>85</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3">
@@ -1420,16 +1404,16 @@
         <v>300</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>24</v>
+        <v>82</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>25</v>
       </c>
       <c r="H2" s="11" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="I2" s="3">
         <v>4</v>
@@ -1441,30 +1425,30 @@
         <v>6</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>63</v>
+        <v>76</v>
       </c>
       <c r="N2" s="5" t="s">
         <v>23</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="Q2" s="3">
         <v>60</v>
       </c>
       <c r="R2" s="4" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:18">
       <c r="A3" s="3" t="s">
-        <v>30</v>
+        <v>86</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3">
@@ -1474,16 +1458,16 @@
         <v>100</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>32</v>
+        <v>74</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>25</v>
       </c>
       <c r="H3" s="13" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="I3" s="3">
         <v>4</v>
@@ -1495,25 +1479,25 @@
         <v>6</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>68</v>
+        <v>84</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="N3" s="5" t="s">
         <v>23</v>
       </c>
       <c r="O3" s="3" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="P3" s="3" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="Q3" s="3">
         <v>60</v>
       </c>
       <c r="R3" s="4" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -1525,8 +1509,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{147B69C7-A702-45C4-913D-71E1B6AF4D13}">
   <dimension ref="A1:S5"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Q14" sqref="Q14"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1569,7 +1553,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>11</v>
@@ -1596,24 +1580,24 @@
         <v>9</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="S1" s="6" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:19">
       <c r="A2" s="3" t="s">
-        <v>29</v>
+        <v>85</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3">
@@ -1623,16 +1607,16 @@
         <v>3</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>24</v>
+        <v>82</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>25</v>
       </c>
       <c r="H2" s="11" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="I2" s="3">
         <v>4</v>
@@ -1644,10 +1628,10 @@
         <v>6</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>64</v>
+        <v>77</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>61</v>
+        <v>76</v>
       </c>
       <c r="N2" s="5" t="s">
         <v>23</v>
@@ -1657,21 +1641,21 @@
         <v>45474</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="Q2" s="3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="R2" s="4" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="S2" s="7" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:19">
       <c r="A3" s="3" t="s">
-        <v>30</v>
+        <v>86</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3">
@@ -1681,16 +1665,16 @@
         <v>1</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>32</v>
+        <v>74</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>25</v>
       </c>
       <c r="H3" s="13" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="I3" s="3">
         <v>1</v>
@@ -1702,10 +1686,10 @@
         <v>1</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>65</v>
+        <v>84</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="N3" s="5" t="s">
         <v>23</v>
@@ -1715,21 +1699,21 @@
         <v>45474</v>
       </c>
       <c r="P3" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q3" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="R3" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="Q3" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="R3" s="4" t="s">
-        <v>49</v>
-      </c>
       <c r="S3" s="7" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:19">
       <c r="A4" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="3">
@@ -1739,16 +1723,16 @@
         <v>1</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>28</v>
+        <v>81</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>25</v>
       </c>
       <c r="H4" s="14" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="I4" s="3">
         <v>1</v>
@@ -1760,10 +1744,10 @@
         <v>1</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>64</v>
+        <v>79</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>66</v>
+        <v>80</v>
       </c>
       <c r="N4" s="5" t="s">
         <v>26</v>
@@ -1773,21 +1757,21 @@
         <v>45474</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="Q4" s="3" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="R4" s="4" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="S4" s="7" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:19">
       <c r="A5" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3">
@@ -1797,16 +1781,16 @@
         <v>1</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>71</v>
+        <v>83</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>25</v>
       </c>
       <c r="H5" s="11" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="I5" s="3">
         <v>1</v>
@@ -1818,10 +1802,10 @@
         <v>1</v>
       </c>
       <c r="L5" s="3" t="s">
-        <v>65</v>
+        <v>84</v>
       </c>
       <c r="M5" s="3" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="N5" s="5" t="s">
         <v>26</v>
@@ -1831,16 +1815,16 @@
         <v>45474</v>
       </c>
       <c r="P5" s="3" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="Q5" s="3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="R5" s="4" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="S5" s="7" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -1853,7 +1837,7 @@
   <dimension ref="A1:O5"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+      <selection activeCell="A2" sqref="A2:A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1892,7 +1876,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>11</v>
@@ -1924,7 +1908,7 @@
     </row>
     <row r="2" spans="1:15">
       <c r="A2" s="3" t="s">
-        <v>29</v>
+        <v>85</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3">
@@ -1934,16 +1918,16 @@
         <v>3</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>24</v>
+        <v>82</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>25</v>
       </c>
       <c r="H2" s="11" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="I2" s="3">
         <v>4</v>
@@ -1955,10 +1939,10 @@
         <v>6</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>64</v>
+        <v>77</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>61</v>
+        <v>76</v>
       </c>
       <c r="N2" s="5" t="s">
         <v>23</v>
@@ -1969,7 +1953,7 @@
     </row>
     <row r="3" spans="1:15">
       <c r="A3" s="3" t="s">
-        <v>30</v>
+        <v>86</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3">
@@ -1979,16 +1963,16 @@
         <v>1</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>32</v>
+        <v>74</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>25</v>
       </c>
       <c r="H3" s="13" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="I3" s="3">
         <v>1</v>
@@ -2000,21 +1984,21 @@
         <v>1</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>65</v>
+        <v>84</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="N3" s="5" t="s">
         <v>23</v>
       </c>
       <c r="O3" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:15">
       <c r="A4" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="3">
@@ -2024,16 +2008,16 @@
         <v>1</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>28</v>
+        <v>81</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>25</v>
       </c>
       <c r="H4" s="14" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="I4" s="3">
         <v>1</v>
@@ -2045,21 +2029,21 @@
         <v>1</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>64</v>
+        <v>79</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>66</v>
+        <v>80</v>
       </c>
       <c r="N4" s="5" t="s">
         <v>26</v>
       </c>
       <c r="O4" s="4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:15">
       <c r="A5" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3">
@@ -2069,16 +2053,16 @@
         <v>1</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>71</v>
+        <v>83</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>25</v>
       </c>
       <c r="H5" s="11" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="I5" s="3">
         <v>1</v>
@@ -2090,16 +2074,16 @@
         <v>1</v>
       </c>
       <c r="L5" s="3" t="s">
-        <v>65</v>
+        <v>84</v>
       </c>
       <c r="M5" s="3" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="N5" s="5" t="s">
         <v>26</v>
       </c>
       <c r="O5" s="4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -2111,8 +2095,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E08C9849-CB54-465E-AADF-08DB0E1F7827}">
   <dimension ref="A1:Z5"/>
   <sheetViews>
-    <sheetView topLeftCell="O1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Y16" sqref="Y16"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -2161,7 +2145,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>11</v>
@@ -2200,7 +2184,7 @@
         <v>18</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="T1" s="1" t="s">
         <v>19</v>
@@ -2212,7 +2196,7 @@
         <v>21</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="X1" s="1" t="s">
         <v>22</v>
@@ -2226,7 +2210,7 @@
     </row>
     <row r="2" spans="1:26">
       <c r="A2" s="3" t="s">
-        <v>29</v>
+        <v>85</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3">
@@ -2239,13 +2223,13 @@
         <v>24</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>25</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="I2" s="3">
         <v>4</v>
@@ -2257,16 +2241,16 @@
         <v>6</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="N2" s="3" t="s">
         <v>23</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="P2" s="3">
         <v>4</v>
@@ -2275,13 +2259,13 @@
         <v>8</v>
       </c>
       <c r="R2" s="3" t="s">
-        <v>71</v>
+        <v>82</v>
       </c>
       <c r="S2" s="3" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="T2" s="3" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="U2" s="3">
         <v>6</v>
@@ -2290,21 +2274,21 @@
         <v>7</v>
       </c>
       <c r="W2" s="3" t="s">
-        <v>65</v>
+        <v>77</v>
       </c>
       <c r="X2" s="3" t="s">
-        <v>31</v>
+        <v>76</v>
       </c>
       <c r="Y2" s="3" t="s">
         <v>26</v>
       </c>
       <c r="Z2" s="3" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:26">
       <c r="A3" s="3" t="s">
-        <v>30</v>
+        <v>86</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3">
@@ -2314,16 +2298,16 @@
         <v>1</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>25</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="I3" s="3">
         <v>1</v>
@@ -2335,16 +2319,16 @@
         <v>1</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="N3" s="3" t="s">
         <v>23</v>
       </c>
       <c r="O3" s="3" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="P3" s="3">
         <v>3</v>
@@ -2353,13 +2337,13 @@
         <v>1</v>
       </c>
       <c r="R3" s="3" t="s">
-        <v>34</v>
+        <v>74</v>
       </c>
       <c r="S3" s="3" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="T3" s="3" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="U3" s="3">
         <v>4</v>
@@ -2368,21 +2352,21 @@
         <v>5</v>
       </c>
       <c r="W3" s="3" t="s">
-        <v>64</v>
+        <v>84</v>
       </c>
       <c r="X3" s="3" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="Y3" s="3" t="s">
         <v>26</v>
       </c>
       <c r="Z3" s="3" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:26">
       <c r="A4" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="3">
@@ -2395,13 +2379,13 @@
         <v>28</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>25</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="I4" s="3">
         <v>1</v>
@@ -2413,16 +2397,16 @@
         <v>1</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="N4" s="3" t="s">
         <v>26</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="P4" s="3">
         <v>0</v>
@@ -2431,13 +2415,13 @@
         <v>2</v>
       </c>
       <c r="R4" s="3" t="s">
-        <v>32</v>
+        <v>81</v>
       </c>
       <c r="S4" s="3" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="T4" s="3" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="U4" s="3">
         <v>5</v>
@@ -2446,21 +2430,21 @@
         <v>6</v>
       </c>
       <c r="W4" s="3" t="s">
-        <v>65</v>
+        <v>79</v>
       </c>
       <c r="X4" s="3" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
       <c r="Y4" s="3" t="s">
         <v>23</v>
       </c>
       <c r="Z4" s="3" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:26">
       <c r="A5" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3">
@@ -2470,37 +2454,37 @@
         <v>1</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>25</v>
       </c>
       <c r="H5" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="I5" s="3">
+        <v>1</v>
+      </c>
+      <c r="J5" s="3">
+        <v>1</v>
+      </c>
+      <c r="K5" s="3">
+        <v>1</v>
+      </c>
+      <c r="L5" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="I5" s="3">
-        <v>1</v>
-      </c>
-      <c r="J5" s="3">
-        <v>1</v>
-      </c>
-      <c r="K5" s="3">
-        <v>1</v>
-      </c>
-      <c r="L5" s="3" t="s">
-        <v>65</v>
-      </c>
       <c r="M5" s="3" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="N5" s="3" t="s">
         <v>26</v>
       </c>
       <c r="O5" s="3" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="P5" s="3">
         <v>0</v>
@@ -2509,13 +2493,13 @@
         <v>1</v>
       </c>
       <c r="R5" s="3" t="s">
-        <v>39</v>
+        <v>83</v>
       </c>
       <c r="S5" s="3" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="T5" s="3" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="U5" s="3">
         <v>5</v>
@@ -2524,16 +2508,16 @@
         <v>6</v>
       </c>
       <c r="W5" s="3" t="s">
-        <v>64</v>
+        <v>84</v>
       </c>
       <c r="X5" s="3" t="s">
-        <v>61</v>
+        <v>78</v>
       </c>
       <c r="Y5" s="3" t="s">
         <v>26</v>
       </c>
       <c r="Z5" s="3" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -2558,13 +2542,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="8" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:3">

</xml_diff>

<commit_message>
change param data driven
</commit_message>
<xml_diff>
--- a/Data/Sheet Metal Part/Order/Order Information (SMP).xlsx
+++ b/Data/Sheet Metal Part/Order/Order Information (SMP).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation Project\gocad-automation-katalon\Data\Sheet Metal Part\Order\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03DC813E-82F9-4F87-B417-1F684D94AA95}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE14BE52-A4C0-42F5-8738-0F69F212D652}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="495" windowWidth="28800" windowHeight="16425" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="495" windowWidth="28800" windowHeight="16425" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FPA011" sheetId="7" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="83">
   <si>
     <t>fileName</t>
   </si>
@@ -220,9 +220,6 @@
     <t>materialGroupChanged</t>
   </si>
   <si>
-    <t>AlMg3-Blech</t>
-  </si>
-  <si>
     <t>115,80</t>
   </si>
   <si>
@@ -253,9 +250,6 @@
     <t>shippingCost</t>
   </si>
   <si>
-    <t>Plasmanitrieren</t>
-  </si>
-  <si>
     <t>Verchromen</t>
   </si>
   <si>
@@ -271,13 +265,16 @@
     <t>stp-testing 3.stp</t>
   </si>
   <si>
-    <t>Standard shipping</t>
-  </si>
-  <si>
-    <t>Pickup at factory</t>
-  </si>
-  <si>
-    <t>Special packaging / via freight forwarding</t>
+    <t>Package delivery (extra costs)</t>
+  </si>
+  <si>
+    <t>Pick-up at factory (no costs)</t>
+  </si>
+  <si>
+    <t>Freight delivery / sepcial packaging (extra costs)</t>
+  </si>
+  <si>
+    <t>EN AW-5754 / AlMg3</t>
   </si>
 </sst>
 </file>
@@ -685,8 +682,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4639641D-1D4F-4B71-AC19-D76CD20CBA7F}">
   <dimension ref="A1:Q5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView topLeftCell="G1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -775,7 +772,7 @@
         <v>2</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>75</v>
+        <v>31</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>54</v>
@@ -808,7 +805,7 @@
         <v>40</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="Q2" s="4" t="s">
         <v>43</v>
@@ -826,7 +823,7 @@
         <v>2</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>54</v>
@@ -850,7 +847,7 @@
         <v>59</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>64</v>
+        <v>82</v>
       </c>
       <c r="N3" s="5" t="s">
         <v>23</v>
@@ -859,7 +856,7 @@
         <v>41</v>
       </c>
       <c r="P3" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="Q3" s="4" t="s">
         <v>43</v>
@@ -877,7 +874,7 @@
         <v>1</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>54</v>
@@ -910,7 +907,7 @@
         <v>42</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="Q4" s="4" t="s">
         <v>43</v>
@@ -928,7 +925,7 @@
         <v>1</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>54</v>
@@ -961,7 +958,7 @@
         <v>40</v>
       </c>
       <c r="P5" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="Q5" s="4" t="s">
         <v>43</v>
@@ -977,8 +974,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DBA0BF0-0221-405C-9926-91F4A4D5B9A2}">
   <dimension ref="A1:S5"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A3"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1060,22 +1057,22 @@
         <v>37</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:19">
       <c r="A2" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3">
         <v>2</v>
       </c>
       <c r="D2" s="3">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>75</v>
+        <v>31</v>
       </c>
       <c r="F2" s="12" t="s">
         <v>54</v>
@@ -1108,7 +1105,7 @@
         <v>40</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="Q2" s="3">
         <v>60</v>
@@ -1122,17 +1119,17 @@
     </row>
     <row r="3" spans="1:19">
       <c r="A3" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3">
         <v>1</v>
       </c>
       <c r="D3" s="3">
-        <v>500</v>
+        <v>200</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F3" s="12" t="s">
         <v>54</v>
@@ -1156,7 +1153,7 @@
         <v>59</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>64</v>
+        <v>82</v>
       </c>
       <c r="N3" s="5" t="s">
         <v>23</v>
@@ -1165,7 +1162,7 @@
         <v>41</v>
       </c>
       <c r="P3" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="Q3" s="3">
         <v>60</v>
@@ -1186,10 +1183,10 @@
         <v>0</v>
       </c>
       <c r="D4" s="3">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F4" s="12" t="s">
         <v>54</v>
@@ -1222,7 +1219,7 @@
         <v>42</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="Q4" s="3">
         <v>60</v>
@@ -1243,10 +1240,10 @@
         <v>0</v>
       </c>
       <c r="D5" s="3">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F5" s="12" t="s">
         <v>54</v>
@@ -1279,7 +1276,7 @@
         <v>40</v>
       </c>
       <c r="P5" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="Q5" s="3">
         <v>60</v>
@@ -1385,7 +1382,7 @@
     </row>
     <row r="2" spans="1:18">
       <c r="A2" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3">
@@ -1395,7 +1392,7 @@
         <v>300</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>75</v>
+        <v>31</v>
       </c>
       <c r="F2" s="12" t="s">
         <v>54</v>
@@ -1428,7 +1425,7 @@
         <v>40</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="Q2" s="3">
         <v>60</v>
@@ -1439,7 +1436,7 @@
     </row>
     <row r="3" spans="1:18">
       <c r="A3" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3">
@@ -1449,7 +1446,7 @@
         <v>100</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F3" s="12" t="s">
         <v>54</v>
@@ -1482,7 +1479,7 @@
         <v>41</v>
       </c>
       <c r="P3" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="Q3" s="3">
         <v>60</v>
@@ -1588,7 +1585,7 @@
     </row>
     <row r="2" spans="1:19">
       <c r="A2" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3">
@@ -1598,7 +1595,7 @@
         <v>3</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>75</v>
+        <v>31</v>
       </c>
       <c r="F2" s="12" t="s">
         <v>54</v>
@@ -1629,24 +1626,24 @@
       </c>
       <c r="O2" s="4">
         <f ca="1">Calculate!$C$2</f>
-        <v>45476</v>
+        <v>45478</v>
       </c>
       <c r="P2" s="3" t="s">
         <v>40</v>
       </c>
       <c r="Q2" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="R2" s="4" t="s">
         <v>43</v>
       </c>
       <c r="S2" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:19">
       <c r="A3" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3">
@@ -1656,7 +1653,7 @@
         <v>1</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F3" s="12" t="s">
         <v>54</v>
@@ -1680,26 +1677,26 @@
         <v>59</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>64</v>
+        <v>82</v>
       </c>
       <c r="N3" s="5" t="s">
         <v>23</v>
       </c>
       <c r="O3" s="4">
         <f ca="1">Calculate!$C$2</f>
-        <v>45476</v>
+        <v>45478</v>
       </c>
       <c r="P3" s="3" t="s">
         <v>41</v>
       </c>
       <c r="Q3" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="R3" s="4" t="s">
         <v>43</v>
       </c>
       <c r="S3" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:19">
@@ -1714,7 +1711,7 @@
         <v>1</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F4" s="12" t="s">
         <v>54</v>
@@ -1745,19 +1742,19 @@
       </c>
       <c r="O4" s="4">
         <f ca="1">Calculate!$C$2</f>
-        <v>45476</v>
+        <v>45478</v>
       </c>
       <c r="P4" s="3" t="s">
         <v>42</v>
       </c>
       <c r="Q4" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="R4" s="4" t="s">
         <v>43</v>
       </c>
       <c r="S4" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:19">
@@ -1772,7 +1769,7 @@
         <v>1</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F5" s="12" t="s">
         <v>54</v>
@@ -1803,19 +1800,19 @@
       </c>
       <c r="O5" s="4">
         <f ca="1">Calculate!$C$2</f>
-        <v>45476</v>
+        <v>45478</v>
       </c>
       <c r="P5" s="3" t="s">
         <v>40</v>
       </c>
       <c r="Q5" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="R5" s="4" t="s">
         <v>43</v>
       </c>
       <c r="S5" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -1899,7 +1896,7 @@
     </row>
     <row r="2" spans="1:15">
       <c r="A2" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3">
@@ -1909,7 +1906,7 @@
         <v>3</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>75</v>
+        <v>31</v>
       </c>
       <c r="F2" s="12" t="s">
         <v>54</v>
@@ -1944,7 +1941,7 @@
     </row>
     <row r="3" spans="1:15">
       <c r="A3" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3">
@@ -1954,7 +1951,7 @@
         <v>1</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F3" s="12" t="s">
         <v>54</v>
@@ -1978,7 +1975,7 @@
         <v>59</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>64</v>
+        <v>82</v>
       </c>
       <c r="N3" s="5" t="s">
         <v>23</v>
@@ -1999,7 +1996,7 @@
         <v>1</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F4" s="12" t="s">
         <v>54</v>
@@ -2044,7 +2041,7 @@
         <v>1</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F5" s="12" t="s">
         <v>54</v>
@@ -2201,7 +2198,7 @@
     </row>
     <row r="2" spans="1:26">
       <c r="A2" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3">
@@ -2211,7 +2208,7 @@
         <v>3</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>75</v>
+        <v>31</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>54</v>
@@ -2241,7 +2238,7 @@
         <v>23</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="P2" s="3">
         <v>4</v>
@@ -2250,7 +2247,7 @@
         <v>8</v>
       </c>
       <c r="R2" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="S2" s="3" t="s">
         <v>54</v>
@@ -2274,12 +2271,12 @@
         <v>25</v>
       </c>
       <c r="Z2" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:26">
       <c r="A3" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3">
@@ -2289,7 +2286,7 @@
         <v>1</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>54</v>
@@ -2319,7 +2316,7 @@
         <v>23</v>
       </c>
       <c r="O3" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="P3" s="3">
         <v>3</v>
@@ -2352,7 +2349,7 @@
         <v>25</v>
       </c>
       <c r="Z3" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:26">
@@ -2367,7 +2364,7 @@
         <v>1</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>54</v>
@@ -2397,7 +2394,7 @@
         <v>25</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="P4" s="3">
         <v>0</v>
@@ -2406,7 +2403,7 @@
         <v>2</v>
       </c>
       <c r="R4" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="S4" s="3" t="s">
         <v>54</v>
@@ -2430,7 +2427,7 @@
         <v>23</v>
       </c>
       <c r="Z4" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:26">
@@ -2445,7 +2442,7 @@
         <v>1</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>54</v>
@@ -2475,7 +2472,7 @@
         <v>25</v>
       </c>
       <c r="O5" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="P5" s="3">
         <v>0</v>
@@ -2508,7 +2505,7 @@
         <v>25</v>
       </c>
       <c r="Z5" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -2545,14 +2542,14 @@
     <row r="2" spans="1:3">
       <c r="A2" s="9">
         <f ca="1">TODAY()</f>
-        <v>45325</v>
+        <v>45327</v>
       </c>
       <c r="B2" s="8">
         <v>5</v>
       </c>
       <c r="C2" s="10">
         <f ca="1">DATE(YEAR(A2),MONTH(A2)+B2,MIN(DAY(A2),DAY(DATE(YEAR(A2),MONTH(A2)+B2+1,0))))</f>
-        <v>45476</v>
+        <v>45478</v>
       </c>
     </row>
   </sheetData>

</xml_diff>